<commit_message>
refresh form after submition
</commit_message>
<xml_diff>
--- a/registration_data.xlsx
+++ b/registration_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,10 +461,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>612203144</t>
-        </is>
+      <c r="A2" t="n">
+        <v>612203144</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -481,9 +479,57 @@
           <t>payalss2004@gmail.com</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>9673095937</t>
+      <c r="E2" t="n">
+        <v>9673095937</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>612203154</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Sakshi</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Khanorkar</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>sakshikhanorkar15@gmail.com</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>1234567890</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>612203142</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Yash</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Pawar</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>yashpawar123@gmail.com</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>1234567890</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Phone number validation implemented
</commit_message>
<xml_diff>
--- a/registration_data.xlsx
+++ b/registration_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="41">
   <si>
     <t>MIS</t>
   </si>
@@ -31,7 +31,13 @@
     <t>Phone</t>
   </si>
   <si>
-    <t>612203127</t>
+    <t>a</t>
+  </si>
+  <si>
+    <t>112103127</t>
+  </si>
+  <si>
+    <t>612203217</t>
   </si>
   <si>
     <t>Payal</t>
@@ -49,12 +55,15 @@
     <t>xyz</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>jabsdi</t>
+  </si>
+  <si>
     <t>Sankpal</t>
   </si>
   <si>
@@ -76,6 +85,12 @@
     <t>P</t>
   </si>
   <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>jkhw</t>
+  </si>
+  <si>
     <t>payalss2004@gmail.com</t>
   </si>
   <si>
@@ -112,7 +127,16 @@
     <t>smruti.pachpute1404@gmail.com</t>
   </si>
   <si>
+    <t>admin@sms.com</t>
+  </si>
+  <si>
     <t>+91 80804 57383</t>
+  </si>
+  <si>
+    <t>1654654</t>
+  </si>
+  <si>
+    <t>987654321</t>
   </si>
 </sst>
 </file>
@@ -470,7 +494,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -498,13 +522,13 @@
         <v>612203144</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E2">
         <v>9673095937</v>
@@ -515,13 +539,13 @@
         <v>612203154</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E3">
         <v>1234567890</v>
@@ -532,13 +556,13 @@
         <v>612203142</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E4">
         <v>1234567890</v>
@@ -549,13 +573,13 @@
         <v>612203127</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E5">
         <v>8080457383</v>
@@ -566,13 +590,13 @@
         <v>1234</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E6">
         <v>1654654</v>
@@ -583,13 +607,13 @@
         <v>1234</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E7">
         <v>54364684561</v>
@@ -600,13 +624,13 @@
         <v>1234</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E8">
         <v>54364684561</v>
@@ -617,13 +641,13 @@
         <v>1234</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E9">
         <v>54364684561</v>
@@ -634,13 +658,13 @@
         <v>1234</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E10">
         <v>54364684561</v>
@@ -651,13 +675,13 @@
         <v>1234</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E11">
         <v>54364684561</v>
@@ -668,13 +692,13 @@
         <v>1234</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E12">
         <v>54364684561</v>
@@ -685,13 +709,13 @@
         <v>1234</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E13">
         <v>1234</v>
@@ -702,13 +726,13 @@
         <v>1234</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E14">
         <v>1234</v>
@@ -719,13 +743,13 @@
         <v>1234</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E15">
         <v>1234</v>
@@ -736,13 +760,13 @@
         <v>1234</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E16">
         <v>1234</v>
@@ -753,13 +777,13 @@
         <v>1234</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D17" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E17">
         <v>1234</v>
@@ -770,13 +794,13 @@
         <v>1234</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D18" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E18">
         <v>8080457383</v>
@@ -787,33 +811,101 @@
         <v>1234</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D19" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E19">
         <v>1654654</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" t="s">
-        <v>5</v>
+      <c r="A20">
+        <v>612203127</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E20" t="s">
-        <v>32</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21">
+        <v>1234</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>